<commit_message>
Módulo 13 - Ferramenta de Análises (atingir metas)
</commit_message>
<xml_diff>
--- a/Módulo 13 - Analise de dados/aula-atingir-meta.xlsx
+++ b/Módulo 13 - Analise de dados/aula-atingir-meta.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bruno\Google Drive\Curso_Excel\12 Ferramentas de análise\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Curso Excel do básico ao avançado\Módulo 13 - Analise de dados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B74C14D-7F1D-45B7-A5F9-BF2CFBF2E043}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{4430C8C5-1BA6-4289-86B7-BC19EE26AF37}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10485" windowHeight="7470"/>
   </bookViews>
   <sheets>
     <sheet name="Atingir Meta" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Público estimado</t>
   </si>
@@ -87,11 +86,76 @@
   <si>
     <t>ATINGIR META</t>
   </si>
+  <si>
+    <t>meta desejada em outra variável.</t>
+  </si>
+  <si>
+    <t>Obs: Só pode ser ajustada uma variável por vez e dependendo do problema pode não existir solução</t>
+  </si>
+  <si>
+    <t>Questões associadas</t>
+  </si>
+  <si>
+    <t>Quanto deve ser o preço do ingresso para chegar ao lucro x desejado?</t>
+  </si>
+  <si>
+    <t>Quanto deve ser o público estimado para chegar ao lucro x desejado?</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Aplicabilidade: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Esta ferramenta permite descobrir o valor ótimo de uma variável para se atingir uma </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Encontrar a ferramenta:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> aba dados/teste de hipóteses/atingir metas/</t>
+    </r>
+  </si>
+  <si>
+    <t>no campo: definir célula insere-se o valor que deseja atingi mediante a meta (resultado/lucro). no campo Para valor insere o valor real que deseja atingir nesse caso colocamos 30.000,00
+e no campo Alternando célula coloca o campo que será manipulado para chegar ao resultado esperado</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="44" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
@@ -202,7 +266,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -251,6 +315,12 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -566,11 +636,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C319CA7F-77A9-4D19-B255-A1F58F239FD6}">
-  <dimension ref="B1:F14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:F32"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23:F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -616,7 +686,7 @@
         <v>2</v>
       </c>
       <c r="C7" s="5">
-        <v>184.87046632124353</v>
+        <v>150</v>
       </c>
       <c r="E7" s="13" t="s">
         <v>5</v>
@@ -630,14 +700,14 @@
         <v>0</v>
       </c>
       <c r="C8" s="6">
-        <v>250</v>
+        <v>500</v>
       </c>
       <c r="E8" s="4" t="s">
         <v>4</v>
       </c>
       <c r="F8" s="5">
         <f>C7*C8</f>
-        <v>46217.616580310882</v>
+        <v>75000</v>
       </c>
     </row>
     <row r="9" spans="2:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -661,7 +731,7 @@
       </c>
       <c r="F10" s="5">
         <f>200*INT(C8/30)</f>
-        <v>1600</v>
+        <v>3200</v>
       </c>
     </row>
     <row r="11" spans="2:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -670,7 +740,7 @@
       </c>
       <c r="F11" s="5">
         <f>3000+(F8*1%)</f>
-        <v>3462.1761658031087</v>
+        <v>3750</v>
       </c>
     </row>
     <row r="12" spans="2:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -679,7 +749,7 @@
       </c>
       <c r="F12" s="5">
         <f>F8*2.5%</f>
-        <v>1155.4404145077722</v>
+        <v>1875</v>
       </c>
     </row>
     <row r="13" spans="2:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -688,16 +758,161 @@
       </c>
       <c r="F13" s="8">
         <f>F8-SUM(F9:F12)</f>
-        <v>15000</v>
+        <v>41175</v>
       </c>
     </row>
     <row r="14" spans="2:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F14" s="1"/>
     </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B17" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="C17" s="17"/>
+      <c r="D17" s="17"/>
+      <c r="E17" s="17"/>
+      <c r="F17" s="17"/>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B18" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="C18" s="17"/>
+      <c r="D18" s="17"/>
+      <c r="E18" s="17"/>
+      <c r="F18" s="17"/>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B19" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="C19" s="17"/>
+      <c r="D19" s="17"/>
+      <c r="E19" s="17"/>
+      <c r="F19" s="17"/>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B20" s="17"/>
+      <c r="C20" s="17"/>
+      <c r="D20" s="17"/>
+      <c r="E20" s="17"/>
+      <c r="F20" s="17"/>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B21" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="C21" s="18"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="18"/>
+      <c r="F21" s="18"/>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B22" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="C22" s="17"/>
+      <c r="D22" s="17"/>
+      <c r="E22" s="17"/>
+      <c r="F22" s="17"/>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B23" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="C23" s="17"/>
+      <c r="D23" s="17"/>
+      <c r="E23" s="17"/>
+      <c r="F23" s="17"/>
+    </row>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B24" s="17"/>
+      <c r="C24" s="17"/>
+      <c r="D24" s="17"/>
+      <c r="E24" s="17"/>
+      <c r="F24" s="17"/>
+    </row>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B25" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="C25" s="17"/>
+      <c r="D25" s="17"/>
+      <c r="E25" s="17"/>
+      <c r="F25" s="17"/>
+    </row>
+    <row r="26" spans="2:6" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="C26" s="17"/>
+      <c r="D26" s="17"/>
+      <c r="E26" s="17"/>
+      <c r="F26" s="17"/>
+    </row>
+    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B27" s="17"/>
+      <c r="C27" s="17"/>
+      <c r="D27" s="17"/>
+      <c r="E27" s="17"/>
+      <c r="F27" s="17"/>
+    </row>
+    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B28" s="17"/>
+      <c r="C28" s="17"/>
+      <c r="D28" s="17"/>
+      <c r="E28" s="17"/>
+      <c r="F28" s="17"/>
+    </row>
+    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B29" s="17"/>
+      <c r="C29" s="17"/>
+      <c r="D29" s="17"/>
+      <c r="E29" s="17"/>
+      <c r="F29" s="17"/>
+    </row>
+    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B30" s="17"/>
+      <c r="C30" s="17"/>
+      <c r="D30" s="17"/>
+      <c r="E30" s="17"/>
+      <c r="F30" s="17"/>
+    </row>
+    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B31" s="17"/>
+      <c r="C31" s="17"/>
+      <c r="D31" s="17"/>
+      <c r="E31" s="17"/>
+      <c r="F31" s="17"/>
+    </row>
+    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B32" s="17"/>
+      <c r="C32" s="17"/>
+      <c r="D32" s="17"/>
+      <c r="E32" s="17"/>
+      <c r="F32" s="17"/>
+    </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="17">
+    <mergeCell ref="B31:F31"/>
+    <mergeCell ref="B32:F32"/>
+    <mergeCell ref="B26:F26"/>
+    <mergeCell ref="B27:F27"/>
+    <mergeCell ref="B28:F28"/>
+    <mergeCell ref="B29:F29"/>
+    <mergeCell ref="B30:F30"/>
+    <mergeCell ref="B21:F21"/>
+    <mergeCell ref="B22:F22"/>
+    <mergeCell ref="B23:F23"/>
+    <mergeCell ref="B24:F24"/>
+    <mergeCell ref="B25:F25"/>
     <mergeCell ref="B1:C1"/>
+    <mergeCell ref="B17:F17"/>
+    <mergeCell ref="B18:F18"/>
+    <mergeCell ref="B19:F19"/>
+    <mergeCell ref="B20:F20"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>